<commit_message>
Newest Files (to 51545)
</commit_message>
<xml_diff>
--- a/icd_files/1104.xlsx
+++ b/icd_files/1104.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\datiphy\Documents\NEO Excel\icd_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586F18D0-2871-453B-A244-AFACD4ADAC07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD17884-5332-4FC4-94F0-299F3356C01C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ADDS Chart" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="381">
   <si>
     <t>CHARTTIME</t>
   </si>
@@ -453,6 +453,9 @@
     <t>02-17</t>
   </si>
   <si>
+    <t>02-18</t>
+  </si>
+  <si>
     <t>02-19</t>
   </si>
   <si>
@@ -468,12 +471,21 @@
     <t>02-23</t>
   </si>
   <si>
+    <t>02-24</t>
+  </si>
+  <si>
+    <t>02-25</t>
+  </si>
+  <si>
     <t>05-15</t>
   </si>
   <si>
     <t>05-16</t>
   </si>
   <si>
+    <t>05-17</t>
+  </si>
+  <si>
     <t>05-18</t>
   </si>
   <si>
@@ -483,6 +495,12 @@
     <t>05-20</t>
   </si>
   <si>
+    <t>05-21</t>
+  </si>
+  <si>
+    <t>08-29</t>
+  </si>
+  <si>
     <t>08-30</t>
   </si>
   <si>
@@ -495,9 +513,15 @@
     <t>09-02</t>
   </si>
   <si>
+    <t>09-05</t>
+  </si>
+  <si>
     <t>09-06</t>
   </si>
   <si>
+    <t>09-07</t>
+  </si>
+  <si>
     <t>GCS: Verbal</t>
   </si>
   <si>
@@ -507,27 +531,231 @@
     <t>GCS: Total</t>
   </si>
   <si>
-    <t>Insulin_x</t>
-  </si>
-  <si>
-    <t>Insulin_y</t>
+    <t>NS</t>
+  </si>
+  <si>
+    <t>Vancomycin</t>
+  </si>
+  <si>
+    <t>Senna</t>
+  </si>
+  <si>
+    <t>Bisacodyl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluticasone-Salmeterol (250/50) </t>
+  </si>
+  <si>
+    <t>Metoclopramide</t>
+  </si>
+  <si>
+    <t>Promethazine HCl</t>
   </si>
   <si>
     <t>Insulin</t>
   </si>
   <si>
+    <t>Terbinafine 1% Cream</t>
+  </si>
+  <si>
+    <t>Lactulose</t>
+  </si>
+  <si>
+    <t>D5W</t>
+  </si>
+  <si>
+    <t>Sodium Chloride 0.9%  Flush</t>
+  </si>
+  <si>
+    <t>Albuterol</t>
+  </si>
+  <si>
+    <t>Warfarin</t>
+  </si>
+  <si>
+    <t>Zolpidem Tartrate</t>
+  </si>
+  <si>
+    <t>0.9% Sodium Chloride</t>
+  </si>
+  <si>
+    <t>Diltiazem Extended-Release</t>
+  </si>
+  <si>
+    <t>Albuterol 0.083% Neb Soln</t>
+  </si>
+  <si>
+    <t>Atorvastatin</t>
+  </si>
+  <si>
+    <t>Glucagon</t>
+  </si>
+  <si>
+    <t>Promethazine</t>
+  </si>
+  <si>
+    <t>Sodium Polystyrene Sulfonate</t>
+  </si>
+  <si>
+    <t>Morphine Sulfate</t>
+  </si>
+  <si>
+    <t>Sodium Chloride Nasal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OxycoDONE (Immediate Release) </t>
+  </si>
+  <si>
+    <t>Iso-Osmotic Dextrose</t>
+  </si>
+  <si>
+    <t>Furosemide</t>
+  </si>
+  <si>
+    <t>Levofloxacin</t>
+  </si>
+  <si>
+    <t>Heparin Sodium</t>
+  </si>
+  <si>
+    <t>Hydrochlorothiazide</t>
+  </si>
+  <si>
+    <t>Metoprolol</t>
+  </si>
+  <si>
+    <t>Oxymetazoline HCl</t>
+  </si>
+  <si>
+    <t>Pantoprazole</t>
+  </si>
+  <si>
+    <t>HYDROmorphone (Dilaudid)</t>
+  </si>
+  <si>
+    <t>NS (Mini Bag Plus)</t>
+  </si>
+  <si>
+    <t>Prochlorperazine</t>
+  </si>
+  <si>
+    <t>Ipratropium Bromide MDI</t>
+  </si>
+  <si>
+    <t>Acetaminophen</t>
+  </si>
+  <si>
+    <t>Ondansetron</t>
+  </si>
+  <si>
+    <t>Sodium Bicarbonate</t>
+  </si>
+  <si>
+    <t>1/2 NS</t>
+  </si>
+  <si>
+    <t>Milk of Magnesia</t>
+  </si>
+  <si>
+    <t>Piperacillin-Tazobactam Na</t>
+  </si>
+  <si>
+    <t>Ipratropium Bromide Neb</t>
+  </si>
+  <si>
+    <t>Ampicillin-Sulbactam</t>
+  </si>
+  <si>
+    <t>Heparin</t>
+  </si>
+  <si>
+    <t>BuPROPion (Sustained Release)</t>
+  </si>
+  <si>
+    <t>NIFEdipine CR</t>
+  </si>
+  <si>
+    <t>Lisinopril</t>
+  </si>
+  <si>
+    <t>Dolasetron Mesylate</t>
+  </si>
+  <si>
     <t>00:00</t>
   </si>
   <si>
+    <t>1000 BAG</t>
+  </si>
+  <si>
     <t>56 ml</t>
   </si>
   <si>
+    <t>3 SYR</t>
+  </si>
+  <si>
+    <t>2-6 SYR</t>
+  </si>
+  <si>
+    <t>100 BAG</t>
+  </si>
+  <si>
+    <t>3 VIAL</t>
+  </si>
+  <si>
+    <t>5000 ml</t>
+  </si>
+  <si>
+    <t>100 TAB</t>
+  </si>
+  <si>
+    <t>100 ml</t>
+  </si>
+  <si>
+    <t>0 VIAL</t>
+  </si>
+  <si>
+    <t>180 CAP</t>
+  </si>
+  <si>
+    <t>1 VIAL</t>
+  </si>
+  <si>
+    <t>180 TAB</t>
+  </si>
+  <si>
+    <t>40 TAB</t>
+  </si>
+  <si>
+    <t>12.5 VIAL</t>
+  </si>
+  <si>
+    <t>200 ml</t>
+  </si>
+  <si>
+    <t>40 VIAL</t>
+  </si>
+  <si>
+    <t>250 TAB</t>
+  </si>
+  <si>
+    <t>25,000 BAG</t>
+  </si>
+  <si>
     <t>17:00</t>
   </si>
   <si>
     <t>19:00</t>
   </si>
   <si>
+    <t>1 DEV</t>
+  </si>
+  <si>
+    <t>7.5 TAB</t>
+  </si>
+  <si>
+    <t>25 TAB</t>
+  </si>
+  <si>
     <t>02:00</t>
   </si>
   <si>
@@ -552,31 +780,118 @@
     <t>20:00</t>
   </si>
   <si>
+    <t>500 TAB</t>
+  </si>
+  <si>
+    <t>5 TAB</t>
+  </si>
+  <si>
+    <t>1-2 SPRY</t>
+  </si>
+  <si>
     <t>62 ml</t>
   </si>
   <si>
-    <t>0 VIAL</t>
+    <t>1 ml</t>
+  </si>
+  <si>
+    <t>10 TAB</t>
+  </si>
+  <si>
+    <t>1-2 INH</t>
+  </si>
+  <si>
+    <t>50 TAB</t>
+  </si>
+  <si>
+    <t>2-4 SYR</t>
+  </si>
+  <si>
+    <t>10 VIAL</t>
+  </si>
+  <si>
+    <t>2 INH</t>
   </si>
   <si>
     <t>52 ml</t>
   </si>
   <si>
+    <t>2 TAB</t>
+  </si>
+  <si>
+    <t>10-20 TAB</t>
+  </si>
+  <si>
+    <t>325-650 TAB</t>
+  </si>
+  <si>
+    <t>4 VIAL</t>
+  </si>
+  <si>
+    <t>650 TAB</t>
+  </si>
+  <si>
+    <t>1000 ml</t>
+  </si>
+  <si>
+    <t>4-8 TAB</t>
+  </si>
+  <si>
+    <t>1000 TAB</t>
+  </si>
+  <si>
+    <t>150 VIAL</t>
+  </si>
+  <si>
+    <t>30 UDCUP</t>
+  </si>
+  <si>
+    <t>1 TAB</t>
+  </si>
+  <si>
+    <t>6.25 AMP</t>
+  </si>
+  <si>
+    <t>1 TUBE</t>
+  </si>
+  <si>
+    <t>2.25 BAG</t>
+  </si>
+  <si>
     <t>16:00</t>
   </si>
   <si>
+    <t>3 TAB</t>
+  </si>
+  <si>
+    <t>1000 mL</t>
+  </si>
+  <si>
+    <t>240 CAP</t>
+  </si>
+  <si>
     <t>62 VIAL</t>
   </si>
   <si>
     <t>32 VIAL</t>
   </si>
   <si>
+    <t>15 BTL</t>
+  </si>
+  <si>
     <t>20 VIAL</t>
   </si>
   <si>
     <t>5 VIAL</t>
   </si>
   <si>
+    <t>2-5 VIAL</t>
+  </si>
+  <si>
     <t>15 VIAL</t>
+  </si>
+  <si>
+    <t>2-4 VIAL</t>
   </si>
   <si>
     <t>Patient Identification Label</t>
@@ -3635,7 +3950,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DDC6-4982-9557-E3D68B4518B0}"/>
+              <c16:uniqueId val="{00000000-001B-4A9A-91C5-B581DECDB9DE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4450,7 +4765,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-DDC6-4982-9557-E3D68B4518B0}"/>
+              <c16:uniqueId val="{00000001-001B-4A9A-91C5-B581DECDB9DE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5265,7 +5580,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-DDC6-4982-9557-E3D68B4518B0}"/>
+              <c16:uniqueId val="{00000002-001B-4A9A-91C5-B581DECDB9DE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6089,7 +6404,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-DDC6-4982-9557-E3D68B4518B0}"/>
+              <c16:uniqueId val="{00000003-001B-4A9A-91C5-B581DECDB9DE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6928,7 +7243,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-DDC6-4982-9557-E3D68B4518B0}"/>
+              <c16:uniqueId val="{00000004-001B-4A9A-91C5-B581DECDB9DE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7476,7 +7791,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-DDC6-4982-9557-E3D68B4518B0}"/>
+              <c16:uniqueId val="{00000005-001B-4A9A-91C5-B581DECDB9DE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7959,7 +8274,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-DDC6-4982-9557-E3D68B4518B0}"/>
+              <c16:uniqueId val="{00000006-001B-4A9A-91C5-B581DECDB9DE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8442,7 +8757,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-DDC6-4982-9557-E3D68B4518B0}"/>
+              <c16:uniqueId val="{00000007-001B-4A9A-91C5-B581DECDB9DE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8925,7 +9240,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-DDC6-4982-9557-E3D68B4518B0}"/>
+              <c16:uniqueId val="{00000008-001B-4A9A-91C5-B581DECDB9DE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -9368,7 +9683,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B244B3A-19CE-420A-84A8-E87645C2ABBF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4854B3-61F5-4F49-B9E2-57A54783C80F}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:AL76"/>
   <sheetViews>
@@ -9393,7 +9708,7 @@
     <row r="1" spans="2:25" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>185</v>
+        <v>290</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -9406,7 +9721,7 @@
     </row>
     <row r="3" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
-        <v>186</v>
+        <v>291</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="10"/>
@@ -9419,7 +9734,7 @@
     </row>
     <row r="4" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
-        <v>187</v>
+        <v>292</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="12"/>
@@ -9432,7 +9747,7 @@
     </row>
     <row r="5" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>188</v>
+        <v>293</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="14"/>
@@ -9445,27 +9760,27 @@
     </row>
     <row r="6" spans="2:25" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="16" t="s">
-        <v>189</v>
+        <v>294</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
       <c r="F6" s="19" t="s">
-        <v>190</v>
+        <v>295</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="21" t="s">
-        <v>191</v>
+        <v>296</v>
       </c>
       <c r="I6" s="20"/>
       <c r="J6" s="22" t="s">
-        <v>192</v>
+        <v>297</v>
       </c>
     </row>
     <row r="7" spans="2:25" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:25" s="29" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>193</v>
+        <v>298</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="25"/>
@@ -9493,7 +9808,7 @@
     </row>
     <row r="9" spans="2:25" s="29" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="30" t="s">
-        <v>194</v>
+        <v>299</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="32"/>
@@ -9521,11 +9836,11 @@
     </row>
     <row r="10" spans="2:25" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="36" t="s">
-        <v>195</v>
+        <v>300</v>
       </c>
       <c r="C10" s="37"/>
       <c r="D10" s="38" t="s">
-        <v>196</v>
+        <v>301</v>
       </c>
       <c r="E10" s="39"/>
       <c r="F10" s="40"/>
@@ -9548,7 +9863,7 @@
       <c r="W10" s="40"/>
       <c r="X10" s="40"/>
       <c r="Y10" s="41" t="s">
-        <v>196</v>
+        <v>301</v>
       </c>
     </row>
     <row r="11" spans="2:25" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9585,7 +9900,7 @@
       <c r="B12" s="42"/>
       <c r="C12" s="43"/>
       <c r="D12" s="48" t="s">
-        <v>197</v>
+        <v>302</v>
       </c>
       <c r="E12" s="49"/>
       <c r="F12" s="50"/>
@@ -9608,14 +9923,14 @@
       <c r="W12" s="50"/>
       <c r="X12" s="50"/>
       <c r="Y12" s="51" t="s">
-        <v>197</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="2:25" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="42"/>
       <c r="C13" s="43"/>
       <c r="D13" s="52" t="s">
-        <v>198</v>
+        <v>303</v>
       </c>
       <c r="E13" s="53"/>
       <c r="F13" s="54"/>
@@ -9638,14 +9953,14 @@
       <c r="W13" s="54"/>
       <c r="X13" s="54"/>
       <c r="Y13" s="55" t="s">
-        <v>198</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="2:25" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="42"/>
       <c r="C14" s="43"/>
       <c r="D14" s="56" t="s">
-        <v>199</v>
+        <v>304</v>
       </c>
       <c r="E14" s="57"/>
       <c r="F14" s="58"/>
@@ -9668,14 +9983,14 @@
       <c r="W14" s="58"/>
       <c r="X14" s="58"/>
       <c r="Y14" s="59" t="s">
-        <v>199</v>
+        <v>304</v>
       </c>
     </row>
     <row r="15" spans="2:25" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="42"/>
       <c r="C15" s="43"/>
       <c r="D15" s="44" t="s">
-        <v>200</v>
+        <v>305</v>
       </c>
       <c r="E15" s="45"/>
       <c r="F15" s="46"/>
@@ -9698,14 +10013,14 @@
       <c r="W15" s="46"/>
       <c r="X15" s="46"/>
       <c r="Y15" s="47" t="s">
-        <v>200</v>
+        <v>305</v>
       </c>
     </row>
     <row r="16" spans="2:25" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="60"/>
       <c r="C16" s="61"/>
       <c r="D16" s="62" t="s">
-        <v>201</v>
+        <v>306</v>
       </c>
       <c r="E16" s="63"/>
       <c r="F16" s="64"/>
@@ -9728,16 +10043,16 @@
       <c r="W16" s="64"/>
       <c r="X16" s="64"/>
       <c r="Y16" s="65" t="s">
-        <v>201</v>
+        <v>306</v>
       </c>
     </row>
     <row r="17" spans="2:38" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="36" t="s">
-        <v>202</v>
+        <v>307</v>
       </c>
       <c r="C17" s="37"/>
       <c r="D17" s="66" t="s">
-        <v>203</v>
+        <v>308</v>
       </c>
       <c r="E17" s="67"/>
       <c r="F17" s="68"/>
@@ -9760,14 +10075,14 @@
       <c r="W17" s="68"/>
       <c r="X17" s="68"/>
       <c r="Y17" s="69" t="s">
-        <v>203</v>
+        <v>308</v>
       </c>
     </row>
     <row r="18" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="42"/>
       <c r="C18" s="43"/>
       <c r="D18" s="52" t="s">
-        <v>204</v>
+        <v>309</v>
       </c>
       <c r="E18" s="53"/>
       <c r="F18" s="54"/>
@@ -9790,10 +10105,10 @@
       <c r="W18" s="54"/>
       <c r="X18" s="54"/>
       <c r="Y18" s="55" t="s">
-        <v>204</v>
+        <v>309</v>
       </c>
       <c r="Z18" s="70" t="s">
-        <v>205</v>
+        <v>310</v>
       </c>
       <c r="AA18" s="71"/>
       <c r="AB18" s="71"/>
@@ -9801,7 +10116,7 @@
       <c r="AD18" s="71"/>
       <c r="AE18" s="72"/>
       <c r="AF18" s="73" t="s">
-        <v>206</v>
+        <v>311</v>
       </c>
       <c r="AG18" s="73"/>
       <c r="AH18" s="73"/>
@@ -9813,7 +10128,7 @@
       <c r="B19" s="60"/>
       <c r="C19" s="61"/>
       <c r="D19" s="75" t="s">
-        <v>207</v>
+        <v>312</v>
       </c>
       <c r="E19" s="76"/>
       <c r="F19" s="77"/>
@@ -9836,7 +10151,7 @@
       <c r="W19" s="77"/>
       <c r="X19" s="77"/>
       <c r="Y19" s="78" t="s">
-        <v>207</v>
+        <v>312</v>
       </c>
       <c r="Z19" s="79"/>
       <c r="AA19" s="80"/>
@@ -9852,11 +10167,11 @@
     </row>
     <row r="20" spans="2:38" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="87" t="s">
-        <v>208</v>
+        <v>313</v>
       </c>
       <c r="C20" s="88"/>
       <c r="D20" s="89" t="s">
-        <v>209</v>
+        <v>314</v>
       </c>
       <c r="E20" s="90"/>
       <c r="F20" s="91"/>
@@ -9879,7 +10194,7 @@
       <c r="W20" s="91"/>
       <c r="X20" s="91"/>
       <c r="Y20" s="92" t="s">
-        <v>209</v>
+        <v>314</v>
       </c>
       <c r="Z20" s="79"/>
       <c r="AA20" s="93"/>
@@ -9897,7 +10212,7 @@
       <c r="B21" s="99"/>
       <c r="C21" s="100"/>
       <c r="D21" s="56" t="s">
-        <v>210</v>
+        <v>315</v>
       </c>
       <c r="E21" s="57"/>
       <c r="F21" s="58"/>
@@ -9920,7 +10235,7 @@
       <c r="W21" s="58"/>
       <c r="X21" s="58"/>
       <c r="Y21" s="59" t="s">
-        <v>210</v>
+        <v>315</v>
       </c>
       <c r="Z21" s="101"/>
       <c r="AA21" s="102"/>
@@ -9939,7 +10254,7 @@
       <c r="B22" s="99"/>
       <c r="C22" s="100"/>
       <c r="D22" s="48" t="s">
-        <v>211</v>
+        <v>316</v>
       </c>
       <c r="E22" s="49"/>
       <c r="F22" s="50"/>
@@ -9962,10 +10277,10 @@
       <c r="W22" s="50"/>
       <c r="X22" s="50"/>
       <c r="Y22" s="51" t="s">
-        <v>211</v>
+        <v>316</v>
       </c>
       <c r="Z22" s="104" t="s">
-        <v>212</v>
+        <v>317</v>
       </c>
       <c r="AA22" s="105"/>
       <c r="AB22" s="105"/>
@@ -9983,7 +10298,7 @@
       <c r="B23" s="107"/>
       <c r="C23" s="108"/>
       <c r="D23" s="109" t="s">
-        <v>213</v>
+        <v>318</v>
       </c>
       <c r="E23" s="110"/>
       <c r="F23" s="111"/>
@@ -10006,52 +10321,52 @@
       <c r="W23" s="111"/>
       <c r="X23" s="111"/>
       <c r="Y23" s="112" t="s">
-        <v>213</v>
+        <v>318</v>
       </c>
       <c r="Z23" s="113" t="s">
-        <v>214</v>
+        <v>319</v>
       </c>
       <c r="AA23" s="77" t="s">
-        <v>215</v>
+        <v>320</v>
       </c>
       <c r="AB23" s="76" t="s">
-        <v>216</v>
+        <v>321</v>
       </c>
       <c r="AC23" s="77" t="s">
-        <v>217</v>
+        <v>322</v>
       </c>
       <c r="AD23" s="76" t="s">
-        <v>218</v>
+        <v>323</v>
       </c>
       <c r="AE23" s="77" t="s">
-        <v>219</v>
+        <v>324</v>
       </c>
       <c r="AF23" s="76" t="s">
-        <v>220</v>
+        <v>325</v>
       </c>
       <c r="AG23" s="77" t="s">
-        <v>221</v>
+        <v>326</v>
       </c>
       <c r="AH23" s="76" t="s">
-        <v>222</v>
+        <v>327</v>
       </c>
       <c r="AI23" s="77" t="s">
-        <v>223</v>
+        <v>328</v>
       </c>
       <c r="AJ23" s="76" t="s">
-        <v>224</v>
+        <v>329</v>
       </c>
       <c r="AK23" s="114" t="s">
-        <v>225</v>
+        <v>330</v>
       </c>
     </row>
     <row r="24" spans="2:38" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="87" t="s">
-        <v>226</v>
+        <v>331</v>
       </c>
       <c r="C24" s="88"/>
       <c r="D24" s="115" t="s">
-        <v>227</v>
+        <v>332</v>
       </c>
       <c r="E24" s="116"/>
       <c r="F24" s="117"/>
@@ -10074,53 +10389,53 @@
       <c r="W24" s="117"/>
       <c r="X24" s="117"/>
       <c r="Y24" s="118" t="s">
-        <v>227</v>
+        <v>332</v>
       </c>
       <c r="Z24" s="119" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AA24" s="120" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AB24" s="121" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AC24" s="122" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AD24" s="123" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AE24" s="124" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AF24" s="123" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AG24" s="125" t="s">
-        <v>231</v>
+        <v>336</v>
       </c>
       <c r="AH24" s="126" t="s">
-        <v>231</v>
+        <v>336</v>
       </c>
       <c r="AI24" s="125" t="s">
-        <v>232</v>
+        <v>337</v>
       </c>
       <c r="AJ24" s="126" t="s">
-        <v>233</v>
+        <v>338</v>
       </c>
       <c r="AK24" s="125" t="s">
-        <v>233</v>
+        <v>338</v>
       </c>
       <c r="AL24" s="127" t="s">
-        <v>234</v>
+        <v>339</v>
       </c>
     </row>
     <row r="25" spans="2:38" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="99"/>
       <c r="C25" s="100"/>
       <c r="D25" s="48" t="s">
-        <v>214</v>
+        <v>319</v>
       </c>
       <c r="E25" s="49"/>
       <c r="F25" s="50"/>
@@ -10143,43 +10458,43 @@
       <c r="W25" s="50"/>
       <c r="X25" s="50"/>
       <c r="Y25" s="51" t="s">
-        <v>214</v>
+        <v>319</v>
       </c>
       <c r="Z25" s="128" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AA25" s="129" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AB25" s="128" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AC25" s="130" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AD25" s="131" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AE25" s="130" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AF25" s="132" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AG25" s="133" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AH25" s="134" t="s">
-        <v>231</v>
+        <v>336</v>
       </c>
       <c r="AI25" s="135" t="s">
-        <v>231</v>
+        <v>336</v>
       </c>
       <c r="AJ25" s="134" t="s">
-        <v>232</v>
+        <v>337</v>
       </c>
       <c r="AK25" s="135" t="s">
-        <v>232</v>
+        <v>337</v>
       </c>
       <c r="AL25" s="136"/>
     </row>
@@ -10187,7 +10502,7 @@
       <c r="B26" s="99"/>
       <c r="C26" s="100"/>
       <c r="D26" s="48" t="s">
-        <v>215</v>
+        <v>320</v>
       </c>
       <c r="E26" s="49"/>
       <c r="F26" s="50"/>
@@ -10210,43 +10525,43 @@
       <c r="W26" s="50"/>
       <c r="X26" s="50"/>
       <c r="Y26" s="51" t="s">
-        <v>215</v>
+        <v>320</v>
       </c>
       <c r="Z26" s="137" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AA26" s="138" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AB26" s="137" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AC26" s="138" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AD26" s="137" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AE26" s="139" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AF26" s="140" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AG26" s="141" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AH26" s="142" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AI26" s="143" t="s">
-        <v>231</v>
+        <v>336</v>
       </c>
       <c r="AJ26" s="144" t="s">
-        <v>231</v>
+        <v>336</v>
       </c>
       <c r="AK26" s="143" t="s">
-        <v>232</v>
+        <v>337</v>
       </c>
       <c r="AL26" s="136"/>
     </row>
@@ -10254,7 +10569,7 @@
       <c r="B27" s="99"/>
       <c r="C27" s="100"/>
       <c r="D27" s="48" t="s">
-        <v>216</v>
+        <v>321</v>
       </c>
       <c r="E27" s="49"/>
       <c r="F27" s="50"/>
@@ -10277,43 +10592,43 @@
       <c r="W27" s="50"/>
       <c r="X27" s="50"/>
       <c r="Y27" s="51" t="s">
-        <v>216</v>
+        <v>321</v>
       </c>
       <c r="Z27" s="145" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AA27" s="146" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AB27" s="147" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AC27" s="146" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AD27" s="147" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AE27" s="148" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AF27" s="149" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AG27" s="150" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AH27" s="151" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AI27" s="152" t="s">
-        <v>231</v>
+        <v>336</v>
       </c>
       <c r="AJ27" s="153" t="s">
-        <v>231</v>
+        <v>336</v>
       </c>
       <c r="AK27" s="152" t="s">
-        <v>231</v>
+        <v>336</v>
       </c>
       <c r="AL27" s="136"/>
     </row>
@@ -10321,7 +10636,7 @@
       <c r="B28" s="99"/>
       <c r="C28" s="100"/>
       <c r="D28" s="154" t="s">
-        <v>217</v>
+        <v>322</v>
       </c>
       <c r="E28" s="53"/>
       <c r="F28" s="54"/>
@@ -10344,43 +10659,43 @@
       <c r="W28" s="54"/>
       <c r="X28" s="54"/>
       <c r="Y28" s="55" t="s">
-        <v>217</v>
+        <v>322</v>
       </c>
       <c r="Z28" s="155" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AA28" s="130" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AB28" s="128" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AC28" s="129" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AD28" s="128" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AE28" s="129" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AF28" s="128" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AG28" s="130" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AH28" s="131" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AI28" s="133" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AJ28" s="132" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AK28" s="133" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AL28" s="136"/>
     </row>
@@ -10388,7 +10703,7 @@
       <c r="B29" s="99"/>
       <c r="C29" s="100"/>
       <c r="D29" s="156" t="s">
-        <v>218</v>
+        <v>323</v>
       </c>
       <c r="E29" s="57"/>
       <c r="F29" s="58"/>
@@ -10411,43 +10726,43 @@
       <c r="W29" s="58"/>
       <c r="X29" s="58"/>
       <c r="Y29" s="59" t="s">
-        <v>218</v>
+        <v>323</v>
       </c>
       <c r="Z29" s="157" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AA29" s="158" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AB29" s="159" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AC29" s="160" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AD29" s="161" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AE29" s="160" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AF29" s="161" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AG29" s="160" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AH29" s="159" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AI29" s="158" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AJ29" s="162" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AK29" s="163" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AL29" s="136"/>
     </row>
@@ -10455,7 +10770,7 @@
       <c r="B30" s="99"/>
       <c r="C30" s="100"/>
       <c r="D30" s="156" t="s">
-        <v>219</v>
+        <v>324</v>
       </c>
       <c r="E30" s="57"/>
       <c r="F30" s="58"/>
@@ -10478,43 +10793,43 @@
       <c r="W30" s="58"/>
       <c r="X30" s="58"/>
       <c r="Y30" s="59" t="s">
-        <v>219</v>
+        <v>324</v>
       </c>
       <c r="Z30" s="164" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AA30" s="148" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AB30" s="149" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AC30" s="148" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AD30" s="147" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AE30" s="146" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AF30" s="147" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AG30" s="146" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AH30" s="147" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AI30" s="148" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AJ30" s="149" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AK30" s="165" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AL30" s="136"/>
     </row>
@@ -10522,7 +10837,7 @@
       <c r="B31" s="99"/>
       <c r="C31" s="100"/>
       <c r="D31" s="156" t="s">
-        <v>220</v>
+        <v>325</v>
       </c>
       <c r="E31" s="57"/>
       <c r="F31" s="58"/>
@@ -10545,43 +10860,43 @@
       <c r="W31" s="58"/>
       <c r="X31" s="58"/>
       <c r="Y31" s="59" t="s">
-        <v>220</v>
+        <v>325</v>
       </c>
       <c r="Z31" s="166" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AA31" s="133" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AB31" s="131" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AC31" s="130" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AD31" s="128" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AE31" s="129" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AF31" s="128" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AG31" s="129" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AH31" s="128" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AI31" s="129" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AJ31" s="128" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AK31" s="167" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AL31" s="136"/>
     </row>
@@ -10589,7 +10904,7 @@
       <c r="B32" s="99"/>
       <c r="C32" s="100"/>
       <c r="D32" s="156" t="s">
-        <v>221</v>
+        <v>326</v>
       </c>
       <c r="E32" s="57"/>
       <c r="F32" s="58"/>
@@ -10612,43 +10927,43 @@
       <c r="W32" s="58"/>
       <c r="X32" s="58"/>
       <c r="Y32" s="59" t="s">
-        <v>221</v>
+        <v>326</v>
       </c>
       <c r="Z32" s="168" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AA32" s="163" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AB32" s="162" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AC32" s="158" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AD32" s="159" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AE32" s="160" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AF32" s="161" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AG32" s="160" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AH32" s="161" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AI32" s="160" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AJ32" s="161" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AK32" s="169" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AL32" s="136"/>
     </row>
@@ -10656,7 +10971,7 @@
       <c r="B33" s="99"/>
       <c r="C33" s="100"/>
       <c r="D33" s="156" t="s">
-        <v>222</v>
+        <v>327</v>
       </c>
       <c r="E33" s="57"/>
       <c r="F33" s="58"/>
@@ -10679,43 +10994,43 @@
       <c r="W33" s="58"/>
       <c r="X33" s="58"/>
       <c r="Y33" s="59" t="s">
-        <v>222</v>
+        <v>327</v>
       </c>
       <c r="Z33" s="170" t="s">
-        <v>231</v>
+        <v>336</v>
       </c>
       <c r="AA33" s="151" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AB33" s="151" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AC33" s="151" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AD33" s="149" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AE33" s="149" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AF33" s="147" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AG33" s="147" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AH33" s="147" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AI33" s="147" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AJ33" s="147" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AK33" s="147" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AL33" s="136"/>
     </row>
@@ -10723,7 +11038,7 @@
       <c r="B34" s="99"/>
       <c r="C34" s="100"/>
       <c r="D34" s="154" t="s">
-        <v>223</v>
+        <v>328</v>
       </c>
       <c r="E34" s="53"/>
       <c r="F34" s="54"/>
@@ -10746,43 +11061,43 @@
       <c r="W34" s="54"/>
       <c r="X34" s="54"/>
       <c r="Y34" s="55" t="s">
-        <v>223</v>
+        <v>328</v>
       </c>
       <c r="Z34" s="171" t="s">
-        <v>231</v>
+        <v>336</v>
       </c>
       <c r="AA34" s="134" t="s">
-        <v>231</v>
+        <v>336</v>
       </c>
       <c r="AB34" s="134" t="s">
-        <v>231</v>
+        <v>336</v>
       </c>
       <c r="AC34" s="132" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AD34" s="132" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AE34" s="132" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AF34" s="131" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AG34" s="131" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AH34" s="128" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AI34" s="128" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AJ34" s="128" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AK34" s="128" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AL34" s="136"/>
     </row>
@@ -10790,7 +11105,7 @@
       <c r="B35" s="99"/>
       <c r="C35" s="100"/>
       <c r="D35" s="48" t="s">
-        <v>224</v>
+        <v>329</v>
       </c>
       <c r="E35" s="49"/>
       <c r="F35" s="50"/>
@@ -10813,43 +11128,43 @@
       <c r="W35" s="50"/>
       <c r="X35" s="50"/>
       <c r="Y35" s="51" t="s">
-        <v>224</v>
+        <v>329</v>
       </c>
       <c r="Z35" s="171" t="s">
-        <v>232</v>
+        <v>337</v>
       </c>
       <c r="AA35" s="134" t="s">
-        <v>231</v>
+        <v>336</v>
       </c>
       <c r="AB35" s="134" t="s">
-        <v>231</v>
+        <v>336</v>
       </c>
       <c r="AC35" s="134" t="s">
-        <v>231</v>
+        <v>336</v>
       </c>
       <c r="AD35" s="132" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AE35" s="132" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AF35" s="132" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AG35" s="132" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="AH35" s="131" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AI35" s="131" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AJ35" s="128" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AK35" s="128" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AL35" s="136"/>
     </row>
@@ -10857,7 +11172,7 @@
       <c r="B36" s="99"/>
       <c r="C36" s="100"/>
       <c r="D36" s="172" t="s">
-        <v>225</v>
+        <v>330</v>
       </c>
       <c r="E36" s="173"/>
       <c r="F36" s="174"/>
@@ -10880,7 +11195,7 @@
       <c r="W36" s="174"/>
       <c r="X36" s="174"/>
       <c r="Y36" s="175" t="s">
-        <v>225</v>
+        <v>330</v>
       </c>
       <c r="Z36" s="176"/>
       <c r="AA36" s="177"/>
@@ -10893,10 +11208,10 @@
       <c r="AH36" s="177"/>
       <c r="AI36" s="177"/>
       <c r="AJ36" s="131" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
       <c r="AK36" s="128" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="AL36" s="136"/>
     </row>
@@ -10904,7 +11219,7 @@
       <c r="B37" s="99"/>
       <c r="C37" s="100"/>
       <c r="D37" s="178" t="s">
-        <v>235</v>
+        <v>340</v>
       </c>
       <c r="E37" s="179"/>
       <c r="F37" s="180"/>
@@ -10927,14 +11242,14 @@
       <c r="W37" s="180"/>
       <c r="X37" s="180"/>
       <c r="Y37" s="181" t="s">
-        <v>235</v>
+        <v>340</v>
       </c>
       <c r="Z37" s="176"/>
       <c r="AA37" s="177"/>
       <c r="AB37" s="177"/>
       <c r="AC37" s="177"/>
       <c r="AD37" s="182" t="s">
-        <v>236</v>
+        <v>341</v>
       </c>
       <c r="AE37" s="182"/>
       <c r="AF37" s="182"/>
@@ -10949,7 +11264,7 @@
       <c r="B38" s="99"/>
       <c r="C38" s="100"/>
       <c r="D38" s="178" t="s">
-        <v>237</v>
+        <v>342</v>
       </c>
       <c r="E38" s="179"/>
       <c r="F38" s="180"/>
@@ -10972,7 +11287,7 @@
       <c r="W38" s="180"/>
       <c r="X38" s="180"/>
       <c r="Y38" s="181" t="s">
-        <v>237</v>
+        <v>342</v>
       </c>
       <c r="Z38" s="176"/>
       <c r="AA38" s="177"/>
@@ -10992,7 +11307,7 @@
       <c r="B39" s="99"/>
       <c r="C39" s="100"/>
       <c r="D39" s="178" t="s">
-        <v>238</v>
+        <v>343</v>
       </c>
       <c r="E39" s="179"/>
       <c r="F39" s="180"/>
@@ -11015,7 +11330,7 @@
       <c r="W39" s="180"/>
       <c r="X39" s="180"/>
       <c r="Y39" s="181" t="s">
-        <v>238</v>
+        <v>343</v>
       </c>
       <c r="Z39" s="176"/>
       <c r="AA39" s="177"/>
@@ -11035,7 +11350,7 @@
       <c r="B40" s="107"/>
       <c r="C40" s="108"/>
       <c r="D40" s="62" t="s">
-        <v>239</v>
+        <v>344</v>
       </c>
       <c r="E40" s="63"/>
       <c r="F40" s="64"/>
@@ -11058,7 +11373,7 @@
       <c r="W40" s="64"/>
       <c r="X40" s="64"/>
       <c r="Y40" s="65" t="s">
-        <v>239</v>
+        <v>344</v>
       </c>
       <c r="Z40" s="185"/>
       <c r="AA40" s="186"/>
@@ -11076,11 +11391,11 @@
     </row>
     <row r="41" spans="2:38" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="87" t="s">
-        <v>240</v>
+        <v>345</v>
       </c>
       <c r="C41" s="88"/>
       <c r="D41" s="38" t="s">
-        <v>241</v>
+        <v>346</v>
       </c>
       <c r="E41" s="39"/>
       <c r="F41" s="40"/>
@@ -11103,14 +11418,14 @@
       <c r="W41" s="40"/>
       <c r="X41" s="40"/>
       <c r="Y41" s="41" t="s">
-        <v>241</v>
+        <v>346</v>
       </c>
     </row>
     <row r="42" spans="2:38" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="99"/>
       <c r="C42" s="100"/>
       <c r="D42" s="44" t="s">
-        <v>220</v>
+        <v>325</v>
       </c>
       <c r="E42" s="45"/>
       <c r="F42" s="46"/>
@@ -11133,14 +11448,14 @@
       <c r="W42" s="46"/>
       <c r="X42" s="46"/>
       <c r="Y42" s="47" t="s">
-        <v>220</v>
+        <v>325</v>
       </c>
     </row>
     <row r="43" spans="2:38" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="99"/>
       <c r="C43" s="100"/>
       <c r="D43" s="48" t="s">
-        <v>221</v>
+        <v>326</v>
       </c>
       <c r="E43" s="49"/>
       <c r="F43" s="50"/>
@@ -11163,14 +11478,14 @@
       <c r="W43" s="50"/>
       <c r="X43" s="50"/>
       <c r="Y43" s="51" t="s">
-        <v>221</v>
+        <v>326</v>
       </c>
     </row>
     <row r="44" spans="2:38" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="99"/>
       <c r="C44" s="100"/>
       <c r="D44" s="48" t="s">
-        <v>222</v>
+        <v>327</v>
       </c>
       <c r="E44" s="49"/>
       <c r="F44" s="50"/>
@@ -11193,14 +11508,14 @@
       <c r="W44" s="50"/>
       <c r="X44" s="50"/>
       <c r="Y44" s="51" t="s">
-        <v>222</v>
+        <v>327</v>
       </c>
     </row>
     <row r="45" spans="2:38" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="99"/>
       <c r="C45" s="100"/>
       <c r="D45" s="52" t="s">
-        <v>223</v>
+        <v>328</v>
       </c>
       <c r="E45" s="53"/>
       <c r="F45" s="54"/>
@@ -11223,14 +11538,14 @@
       <c r="W45" s="54"/>
       <c r="X45" s="54"/>
       <c r="Y45" s="55" t="s">
-        <v>223</v>
+        <v>328</v>
       </c>
     </row>
     <row r="46" spans="2:38" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="99"/>
       <c r="C46" s="100"/>
       <c r="D46" s="56" t="s">
-        <v>224</v>
+        <v>329</v>
       </c>
       <c r="E46" s="57"/>
       <c r="F46" s="58"/>
@@ -11253,14 +11568,14 @@
       <c r="W46" s="58"/>
       <c r="X46" s="58"/>
       <c r="Y46" s="59" t="s">
-        <v>224</v>
+        <v>329</v>
       </c>
     </row>
     <row r="47" spans="2:38" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="99"/>
       <c r="C47" s="100"/>
       <c r="D47" s="56" t="s">
-        <v>225</v>
+        <v>330</v>
       </c>
       <c r="E47" s="57"/>
       <c r="F47" s="58"/>
@@ -11283,10 +11598,10 @@
       <c r="W47" s="58"/>
       <c r="X47" s="58"/>
       <c r="Y47" s="59" t="s">
-        <v>225</v>
+        <v>330</v>
       </c>
       <c r="AA47" s="189" t="s">
-        <v>242</v>
+        <v>347</v>
       </c>
       <c r="AB47" s="190"/>
       <c r="AC47" s="190"/>
@@ -11303,7 +11618,7 @@
       <c r="B48" s="99"/>
       <c r="C48" s="100"/>
       <c r="D48" s="56" t="s">
-        <v>235</v>
+        <v>340</v>
       </c>
       <c r="E48" s="57"/>
       <c r="F48" s="58"/>
@@ -11326,7 +11641,7 @@
       <c r="W48" s="58"/>
       <c r="X48" s="58"/>
       <c r="Y48" s="59" t="s">
-        <v>235</v>
+        <v>340</v>
       </c>
       <c r="AA48" s="190"/>
       <c r="AB48" s="190"/>
@@ -11344,7 +11659,7 @@
       <c r="B49" s="99"/>
       <c r="C49" s="100"/>
       <c r="D49" s="56" t="s">
-        <v>237</v>
+        <v>342</v>
       </c>
       <c r="E49" s="57"/>
       <c r="F49" s="58"/>
@@ -11367,7 +11682,7 @@
       <c r="W49" s="58"/>
       <c r="X49" s="58"/>
       <c r="Y49" s="59" t="s">
-        <v>237</v>
+        <v>342</v>
       </c>
       <c r="AA49" s="190"/>
       <c r="AB49" s="190"/>
@@ -11385,7 +11700,7 @@
       <c r="B50" s="99"/>
       <c r="C50" s="100"/>
       <c r="D50" s="56" t="s">
-        <v>238</v>
+        <v>343</v>
       </c>
       <c r="E50" s="57"/>
       <c r="F50" s="58"/>
@@ -11408,14 +11723,14 @@
       <c r="W50" s="58"/>
       <c r="X50" s="58"/>
       <c r="Y50" s="59" t="s">
-        <v>238</v>
+        <v>343</v>
       </c>
     </row>
     <row r="51" spans="2:37" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="99"/>
       <c r="C51" s="100"/>
       <c r="D51" s="52" t="s">
-        <v>239</v>
+        <v>344</v>
       </c>
       <c r="E51" s="53"/>
       <c r="F51" s="54"/>
@@ -11438,14 +11753,14 @@
       <c r="W51" s="54"/>
       <c r="X51" s="54"/>
       <c r="Y51" s="55" t="s">
-        <v>239</v>
+        <v>344</v>
       </c>
     </row>
     <row r="52" spans="2:37" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="107"/>
       <c r="C52" s="108"/>
       <c r="D52" s="62" t="s">
-        <v>243</v>
+        <v>348</v>
       </c>
       <c r="E52" s="63"/>
       <c r="F52" s="64"/>
@@ -11468,24 +11783,24 @@
       <c r="W52" s="64"/>
       <c r="X52" s="64"/>
       <c r="Y52" s="65" t="s">
-        <v>243</v>
+        <v>348</v>
       </c>
       <c r="AB52" s="191"/>
       <c r="AC52" s="191"/>
       <c r="AD52" s="191"/>
       <c r="AE52" s="191"/>
       <c r="AG52" s="14" t="s">
-        <v>244</v>
+        <v>349</v>
       </c>
       <c r="AH52" s="14"/>
     </row>
     <row r="53" spans="2:37" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="36" t="s">
-        <v>245</v>
+        <v>350</v>
       </c>
       <c r="C53" s="37"/>
       <c r="D53" s="66" t="s">
-        <v>246</v>
+        <v>351</v>
       </c>
       <c r="E53" s="67"/>
       <c r="F53" s="68"/>
@@ -11508,7 +11823,7 @@
       <c r="W53" s="68"/>
       <c r="X53" s="68"/>
       <c r="Y53" s="69" t="s">
-        <v>246</v>
+        <v>351</v>
       </c>
       <c r="AG53" s="192"/>
       <c r="AH53" s="192"/>
@@ -11517,7 +11832,7 @@
       <c r="B54" s="42"/>
       <c r="C54" s="43"/>
       <c r="D54" s="52" t="s">
-        <v>247</v>
+        <v>352</v>
       </c>
       <c r="E54" s="53"/>
       <c r="F54" s="54"/>
@@ -11540,14 +11855,14 @@
       <c r="W54" s="54"/>
       <c r="X54" s="54"/>
       <c r="Y54" s="55" t="s">
-        <v>247</v>
+        <v>352</v>
       </c>
       <c r="AB54" s="193"/>
       <c r="AC54" s="193"/>
       <c r="AD54" s="193"/>
       <c r="AE54" s="193"/>
       <c r="AG54" s="14" t="s">
-        <v>248</v>
+        <v>353</v>
       </c>
       <c r="AH54" s="14"/>
     </row>
@@ -11555,7 +11870,7 @@
       <c r="B55" s="42"/>
       <c r="C55" s="43"/>
       <c r="D55" s="56" t="s">
-        <v>249</v>
+        <v>354</v>
       </c>
       <c r="E55" s="57"/>
       <c r="F55" s="58"/>
@@ -11578,7 +11893,7 @@
       <c r="W55" s="58"/>
       <c r="X55" s="58"/>
       <c r="Y55" s="59" t="s">
-        <v>249</v>
+        <v>354</v>
       </c>
       <c r="AG55" s="192"/>
       <c r="AH55" s="192"/>
@@ -11587,7 +11902,7 @@
       <c r="B56" s="42"/>
       <c r="C56" s="43"/>
       <c r="D56" s="52" t="s">
-        <v>250</v>
+        <v>355</v>
       </c>
       <c r="E56" s="53"/>
       <c r="F56" s="54"/>
@@ -11610,14 +11925,14 @@
       <c r="W56" s="54"/>
       <c r="X56" s="54"/>
       <c r="Y56" s="55" t="s">
-        <v>250</v>
+        <v>355</v>
       </c>
       <c r="AB56" s="194"/>
       <c r="AC56" s="194"/>
       <c r="AD56" s="194"/>
       <c r="AE56" s="194"/>
       <c r="AG56" s="14" t="s">
-        <v>251</v>
+        <v>356</v>
       </c>
       <c r="AH56" s="14"/>
     </row>
@@ -11625,7 +11940,7 @@
       <c r="B57" s="42"/>
       <c r="C57" s="43"/>
       <c r="D57" s="48" t="s">
-        <v>252</v>
+        <v>357</v>
       </c>
       <c r="E57" s="49"/>
       <c r="F57" s="50"/>
@@ -11648,7 +11963,7 @@
       <c r="W57" s="50"/>
       <c r="X57" s="50"/>
       <c r="Y57" s="51" t="s">
-        <v>252</v>
+        <v>357</v>
       </c>
       <c r="AG57" s="192"/>
       <c r="AH57" s="192"/>
@@ -11657,7 +11972,7 @@
       <c r="B58" s="60"/>
       <c r="C58" s="61"/>
       <c r="D58" s="109" t="s">
-        <v>253</v>
+        <v>358</v>
       </c>
       <c r="E58" s="110"/>
       <c r="F58" s="111"/>
@@ -11680,24 +11995,24 @@
       <c r="W58" s="111"/>
       <c r="X58" s="111"/>
       <c r="Y58" s="112" t="s">
-        <v>253</v>
+        <v>358</v>
       </c>
       <c r="AB58" s="195"/>
       <c r="AC58" s="195"/>
       <c r="AD58" s="195"/>
       <c r="AE58" s="195"/>
       <c r="AG58" s="14" t="s">
-        <v>254</v>
+        <v>359</v>
       </c>
       <c r="AH58" s="14"/>
     </row>
     <row r="59" spans="2:37" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="36" t="s">
-        <v>255</v>
+        <v>360</v>
       </c>
       <c r="C59" s="37"/>
       <c r="D59" s="196" t="s">
-        <v>256</v>
+        <v>361</v>
       </c>
       <c r="E59" s="197"/>
       <c r="F59" s="198"/>
@@ -11720,7 +12035,7 @@
       <c r="W59" s="198"/>
       <c r="X59" s="198"/>
       <c r="Y59" s="199" t="s">
-        <v>256</v>
+        <v>361</v>
       </c>
       <c r="AG59" s="192"/>
       <c r="AH59" s="192"/>
@@ -11729,7 +12044,7 @@
       <c r="B60" s="42"/>
       <c r="C60" s="43"/>
       <c r="D60" s="56" t="s">
-        <v>257</v>
+        <v>362</v>
       </c>
       <c r="E60" s="57"/>
       <c r="F60" s="58"/>
@@ -11752,22 +12067,22 @@
       <c r="W60" s="58"/>
       <c r="X60" s="58"/>
       <c r="Y60" s="59" t="s">
-        <v>257</v>
+        <v>362</v>
       </c>
       <c r="AB60" s="135" t="s">
-        <v>232</v>
+        <v>337</v>
       </c>
       <c r="AC60" s="135" t="s">
-        <v>232</v>
+        <v>337</v>
       </c>
       <c r="AD60" s="135" t="s">
-        <v>232</v>
+        <v>337</v>
       </c>
       <c r="AE60" s="135" t="s">
-        <v>232</v>
+        <v>337</v>
       </c>
       <c r="AG60" s="14" t="s">
-        <v>258</v>
+        <v>363</v>
       </c>
       <c r="AH60" s="14"/>
     </row>
@@ -11775,7 +12090,7 @@
       <c r="B61" s="42"/>
       <c r="C61" s="43"/>
       <c r="D61" s="48" t="s">
-        <v>259</v>
+        <v>364</v>
       </c>
       <c r="E61" s="49"/>
       <c r="F61" s="50"/>
@@ -11798,7 +12113,7 @@
       <c r="W61" s="50"/>
       <c r="X61" s="50"/>
       <c r="Y61" s="51" t="s">
-        <v>259</v>
+        <v>364</v>
       </c>
       <c r="AB61" s="200"/>
       <c r="AC61" s="200"/>
@@ -11811,7 +12126,7 @@
       <c r="B62" s="60"/>
       <c r="C62" s="61"/>
       <c r="D62" s="109" t="s">
-        <v>260</v>
+        <v>365</v>
       </c>
       <c r="E62" s="110"/>
       <c r="F62" s="111"/>
@@ -11834,32 +12149,32 @@
       <c r="W62" s="111"/>
       <c r="X62" s="111"/>
       <c r="Y62" s="112" t="s">
-        <v>260</v>
+        <v>365</v>
       </c>
       <c r="AB62" s="135" t="s">
-        <v>233</v>
+        <v>338</v>
       </c>
       <c r="AC62" s="135" t="s">
-        <v>233</v>
+        <v>338</v>
       </c>
       <c r="AD62" s="135" t="s">
-        <v>233</v>
+        <v>338</v>
       </c>
       <c r="AE62" s="135" t="s">
-        <v>233</v>
+        <v>338</v>
       </c>
       <c r="AG62" s="14" t="s">
-        <v>261</v>
+        <v>366</v>
       </c>
       <c r="AH62" s="14"/>
     </row>
     <row r="63" spans="2:37" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="36" t="s">
-        <v>262</v>
+        <v>367</v>
       </c>
       <c r="C63" s="37"/>
       <c r="D63" s="89" t="s">
-        <v>263</v>
+        <v>368</v>
       </c>
       <c r="E63" s="90"/>
       <c r="F63" s="91"/>
@@ -11882,7 +12197,7 @@
       <c r="W63" s="91"/>
       <c r="X63" s="91"/>
       <c r="Y63" s="92" t="s">
-        <v>263</v>
+        <v>368</v>
       </c>
       <c r="AG63" s="192"/>
       <c r="AH63" s="192"/>
@@ -11891,7 +12206,7 @@
       <c r="B64" s="42"/>
       <c r="C64" s="43"/>
       <c r="D64" s="52" t="s">
-        <v>264</v>
+        <v>369</v>
       </c>
       <c r="E64" s="53"/>
       <c r="F64" s="54"/>
@@ -11914,14 +12229,14 @@
       <c r="W64" s="54"/>
       <c r="X64" s="54"/>
       <c r="Y64" s="55" t="s">
-        <v>264</v>
+        <v>369</v>
       </c>
       <c r="AB64" s="201"/>
       <c r="AC64" s="201"/>
       <c r="AD64" s="201"/>
       <c r="AE64" s="201"/>
       <c r="AG64" s="14" t="s">
-        <v>265</v>
+        <v>370</v>
       </c>
       <c r="AH64" s="14"/>
     </row>
@@ -11929,7 +12244,7 @@
       <c r="B65" s="42"/>
       <c r="C65" s="43"/>
       <c r="D65" s="44" t="s">
-        <v>266</v>
+        <v>371</v>
       </c>
       <c r="E65" s="45"/>
       <c r="F65" s="46"/>
@@ -11952,14 +12267,14 @@
       <c r="W65" s="46"/>
       <c r="X65" s="46"/>
       <c r="Y65" s="47" t="s">
-        <v>266</v>
+        <v>371</v>
       </c>
     </row>
     <row r="66" spans="2:25" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="60"/>
       <c r="C66" s="61"/>
       <c r="D66" s="62" t="s">
-        <v>267</v>
+        <v>372</v>
       </c>
       <c r="E66" s="63"/>
       <c r="F66" s="64"/>
@@ -11982,12 +12297,12 @@
       <c r="W66" s="64"/>
       <c r="X66" s="64"/>
       <c r="Y66" s="65" t="s">
-        <v>267</v>
+        <v>372</v>
       </c>
     </row>
     <row r="67" spans="2:25" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="202" t="s">
-        <v>268</v>
+        <v>373</v>
       </c>
       <c r="C67" s="203"/>
       <c r="D67" s="204"/>
@@ -12015,7 +12330,7 @@
     </row>
     <row r="68" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="208" t="s">
-        <v>269</v>
+        <v>374</v>
       </c>
       <c r="C68" s="209" t="s">
         <v>4</v>
@@ -12042,13 +12357,13 @@
       <c r="W68" s="91"/>
       <c r="X68" s="91"/>
       <c r="Y68" s="211" t="s">
-        <v>270</v>
+        <v>375</v>
       </c>
     </row>
     <row r="69" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="212"/>
       <c r="C69" s="213" t="s">
-        <v>271</v>
+        <v>376</v>
       </c>
       <c r="D69" s="214"/>
       <c r="E69" s="57"/>
@@ -12076,7 +12391,7 @@
     <row r="70" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="212"/>
       <c r="C70" s="213" t="s">
-        <v>272</v>
+        <v>377</v>
       </c>
       <c r="D70" s="214"/>
       <c r="E70" s="57"/>
@@ -12188,7 +12503,7 @@
     <row r="74" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="212"/>
       <c r="C74" s="213" t="s">
-        <v>273</v>
+        <v>378</v>
       </c>
       <c r="D74" s="214"/>
       <c r="E74" s="57"/>
@@ -12216,7 +12531,7 @@
     <row r="75" spans="2:25" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B75" s="212"/>
       <c r="C75" s="213" t="s">
-        <v>274</v>
+        <v>379</v>
       </c>
       <c r="D75" s="214"/>
       <c r="E75" s="216"/>
@@ -12244,7 +12559,7 @@
     <row r="76" spans="2:25" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B76" s="218"/>
       <c r="C76" s="219" t="s">
-        <v>275</v>
+        <v>380</v>
       </c>
       <c r="D76" s="220"/>
       <c r="E76" s="221"/>
@@ -15396,13 +15711,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A30:BD38"/>
+  <dimension ref="A30:CL85"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="30" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>140</v>
       </c>
@@ -15410,117 +15725,117 @@
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:90" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>142</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="M31" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="N31" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="O31" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="N31" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="O31" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="P31" s="1" t="s">
         <v>145</v>
       </c>
       <c r="Q31" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="U31" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="V31" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="W31" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="R31" s="1" t="s">
+      <c r="X31" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="S31" s="1" t="s">
+      <c r="Y31" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="T31" s="1" t="s">
+      <c r="Z31" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="U31" s="1" t="s">
+      <c r="AA31" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AB31" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC31" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AD31" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="V31" s="1" t="s">
+      <c r="AE31" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AF31" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AG31" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AH31" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AI31" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="W31" s="1" t="s">
+      <c r="AJ31" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="X31" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="Y31" s="1" t="s">
+      <c r="AK31" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="Z31" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="AA31" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="AB31" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="AC31" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="AD31" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="AE31" s="1" t="s">
+      <c r="AL31" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="AF31" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="AG31" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="AH31" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="AI31" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="AJ31" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="AK31" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="AL31" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="AM31" s="1" t="s">
         <v>151</v>
@@ -15532,267 +15847,438 @@
         <v>151</v>
       </c>
       <c r="AP31" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AQ31" s="1" t="s">
         <v>152</v>
       </c>
       <c r="AR31" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AS31" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AT31" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AU31" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AV31" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AW31" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AX31" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AY31" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AZ31" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="AS31" s="1" t="s">
+      <c r="BA31" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="AT31" s="1" t="s">
+      <c r="BB31" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="AU31" s="1" t="s">
+      <c r="BC31" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="BD31" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="AV31" s="1" t="s">
+      <c r="BE31" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="AW31" s="1" t="s">
+      <c r="BF31" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="BG31" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="BH31" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="BI31" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="BJ31" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="BK31" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AX31" s="1" t="s">
+      <c r="BL31" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AY31" s="1" t="s">
+      <c r="BM31" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AZ31" s="1" t="s">
+      <c r="BN31" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="BA31" s="1" t="s">
+      <c r="BO31" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="BB31" s="1" t="s">
+      <c r="BP31" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="BC31" s="1" t="s">
+      <c r="BQ31" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="BR31" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="BD31" s="1" t="s">
+      <c r="BS31" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BT31" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="32" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="BU31" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="BV31" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BW31" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BX31" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BY31" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BZ31" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="CA31" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="CB31" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="CC31" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="CD31" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="CE31" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="CF31" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="CG31" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="CH31" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="CI31" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="CJ31" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="CK31" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="CL31" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>164</v>
+        <v>219</v>
       </c>
       <c r="C32" t="s">
+        <v>219</v>
+      </c>
+      <c r="D32" t="s">
+        <v>219</v>
+      </c>
+      <c r="E32" t="s">
+        <v>219</v>
+      </c>
+      <c r="F32" t="s">
+        <v>219</v>
+      </c>
+      <c r="G32" t="s">
+        <v>219</v>
+      </c>
+      <c r="H32" t="s">
+        <v>219</v>
+      </c>
+      <c r="I32" t="s">
+        <v>219</v>
+      </c>
+      <c r="J32" t="s">
+        <v>219</v>
+      </c>
+      <c r="K32" t="s">
+        <v>219</v>
+      </c>
+      <c r="L32" t="s">
+        <v>219</v>
+      </c>
+      <c r="M32" t="s">
+        <v>219</v>
+      </c>
+      <c r="N32" t="s">
+        <v>239</v>
+      </c>
+      <c r="O32" t="s">
+        <v>240</v>
+      </c>
+      <c r="P32" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>244</v>
+      </c>
+      <c r="R32" t="s">
+        <v>245</v>
+      </c>
+      <c r="S32" t="s">
+        <v>246</v>
+      </c>
+      <c r="T32" t="s">
+        <v>247</v>
+      </c>
+      <c r="U32" t="s">
+        <v>240</v>
+      </c>
+      <c r="V32" t="s">
+        <v>248</v>
+      </c>
+      <c r="W32" t="s">
+        <v>219</v>
+      </c>
+      <c r="X32" t="s">
+        <v>249</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>250</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>247</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>251</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>248</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>219</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>250</v>
+      </c>
+      <c r="AF32" t="s">
+        <v>246</v>
+      </c>
+      <c r="AG32" t="s">
+        <v>247</v>
+      </c>
+      <c r="AH32" t="s">
+        <v>240</v>
+      </c>
+      <c r="AI32" t="s">
+        <v>219</v>
+      </c>
+      <c r="AJ32" t="s">
+        <v>219</v>
+      </c>
+      <c r="AK32" t="s">
+        <v>219</v>
+      </c>
+      <c r="AL32" t="s">
+        <v>219</v>
+      </c>
+      <c r="AM32" t="s">
+        <v>219</v>
+      </c>
+      <c r="AN32" t="s">
+        <v>219</v>
+      </c>
+      <c r="AO32" t="s">
+        <v>219</v>
+      </c>
+      <c r="AP32" t="s">
+        <v>219</v>
+      </c>
+      <c r="AQ32" t="s">
+        <v>219</v>
+      </c>
+      <c r="AR32" t="s">
+        <v>219</v>
+      </c>
+      <c r="AS32" t="s">
+        <v>219</v>
+      </c>
+      <c r="AT32" t="s">
+        <v>219</v>
+      </c>
+      <c r="AU32" t="s">
+        <v>219</v>
+      </c>
+      <c r="AV32" t="s">
+        <v>219</v>
+      </c>
+      <c r="AW32" t="s">
+        <v>219</v>
+      </c>
+      <c r="AX32" t="s">
+        <v>219</v>
+      </c>
+      <c r="AY32" t="s">
+        <v>219</v>
+      </c>
+      <c r="AZ32" t="s">
+        <v>219</v>
+      </c>
+      <c r="BA32" t="s">
+        <v>219</v>
+      </c>
+      <c r="BB32" t="s">
+        <v>219</v>
+      </c>
+      <c r="BC32" t="s">
+        <v>219</v>
+      </c>
+      <c r="BD32" t="s">
+        <v>219</v>
+      </c>
+      <c r="BE32" t="s">
+        <v>219</v>
+      </c>
+      <c r="BF32" t="s">
+        <v>245</v>
+      </c>
+      <c r="BG32" t="s">
+        <v>246</v>
+      </c>
+      <c r="BH32" t="s">
+        <v>278</v>
+      </c>
+      <c r="BI32" t="s">
+        <v>240</v>
+      </c>
+      <c r="BJ32" t="s">
+        <v>248</v>
+      </c>
+      <c r="BK32" t="s">
+        <v>219</v>
+      </c>
+      <c r="BL32" t="s">
+        <v>249</v>
+      </c>
+      <c r="BM32" t="s">
+        <v>250</v>
+      </c>
+      <c r="BN32" t="s">
+        <v>246</v>
+      </c>
+      <c r="BO32" t="s">
+        <v>247</v>
+      </c>
+      <c r="BP32" t="s">
+        <v>240</v>
+      </c>
+      <c r="BQ32" t="s">
+        <v>248</v>
+      </c>
+      <c r="BR32" t="s">
+        <v>219</v>
+      </c>
+      <c r="BS32" t="s">
+        <v>250</v>
+      </c>
+      <c r="BT32" t="s">
+        <v>219</v>
+      </c>
+      <c r="BU32" t="s">
+        <v>219</v>
+      </c>
+      <c r="BV32" t="s">
+        <v>219</v>
+      </c>
+      <c r="BW32" t="s">
+        <v>219</v>
+      </c>
+      <c r="BX32" t="s">
+        <v>219</v>
+      </c>
+      <c r="BY32" t="s">
+        <v>219</v>
+      </c>
+      <c r="BZ32" t="s">
+        <v>219</v>
+      </c>
+      <c r="CA32" t="s">
+        <v>219</v>
+      </c>
+      <c r="CB32" t="s">
+        <v>219</v>
+      </c>
+      <c r="CC32" t="s">
+        <v>219</v>
+      </c>
+      <c r="CD32" t="s">
+        <v>219</v>
+      </c>
+      <c r="CE32" t="s">
+        <v>219</v>
+      </c>
+      <c r="CF32" t="s">
+        <v>219</v>
+      </c>
+      <c r="CG32" t="s">
+        <v>219</v>
+      </c>
+      <c r="CH32" t="s">
+        <v>219</v>
+      </c>
+      <c r="CI32" t="s">
+        <v>219</v>
+      </c>
+      <c r="CJ32" t="s">
+        <v>219</v>
+      </c>
+      <c r="CK32" t="s">
+        <v>219</v>
+      </c>
+      <c r="CL32" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="33" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D32" t="s">
+    </row>
+    <row r="34" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E32" t="s">
+    </row>
+    <row r="35" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="F32" t="s">
-        <v>169</v>
-      </c>
-      <c r="G32" t="s">
-        <v>170</v>
-      </c>
-      <c r="H32" t="s">
-        <v>171</v>
-      </c>
-      <c r="I32" t="s">
-        <v>167</v>
-      </c>
-      <c r="J32" t="s">
-        <v>172</v>
-      </c>
-      <c r="K32" t="s">
-        <v>173</v>
-      </c>
-      <c r="L32" t="s">
-        <v>174</v>
-      </c>
-      <c r="M32" t="s">
-        <v>170</v>
-      </c>
-      <c r="N32" t="s">
-        <v>171</v>
-      </c>
-      <c r="O32" t="s">
-        <v>175</v>
-      </c>
-      <c r="P32" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>174</v>
-      </c>
-      <c r="R32" t="s">
-        <v>170</v>
-      </c>
-      <c r="S32" t="s">
-        <v>171</v>
-      </c>
-      <c r="T32" t="s">
-        <v>167</v>
-      </c>
-      <c r="U32" t="s">
-        <v>164</v>
-      </c>
-      <c r="V32" t="s">
-        <v>164</v>
-      </c>
-      <c r="W32" t="s">
-        <v>164</v>
-      </c>
-      <c r="X32" t="s">
-        <v>164</v>
-      </c>
-      <c r="Y32" t="s">
-        <v>164</v>
-      </c>
-      <c r="Z32" t="s">
-        <v>164</v>
-      </c>
-      <c r="AA32" t="s">
-        <v>164</v>
-      </c>
-      <c r="AB32" t="s">
-        <v>164</v>
-      </c>
-      <c r="AC32" t="s">
-        <v>164</v>
-      </c>
-      <c r="AD32" t="s">
-        <v>164</v>
-      </c>
-      <c r="AE32" t="s">
-        <v>164</v>
-      </c>
-      <c r="AF32" t="s">
-        <v>169</v>
-      </c>
-      <c r="AG32" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH32" t="s">
-        <v>179</v>
-      </c>
-      <c r="AI32" t="s">
-        <v>167</v>
-      </c>
-      <c r="AJ32" t="s">
-        <v>172</v>
-      </c>
-      <c r="AK32" t="s">
-        <v>173</v>
-      </c>
-      <c r="AL32" t="s">
-        <v>174</v>
-      </c>
-      <c r="AM32" t="s">
-        <v>170</v>
-      </c>
-      <c r="AN32" t="s">
-        <v>171</v>
-      </c>
-      <c r="AO32" t="s">
-        <v>167</v>
-      </c>
-      <c r="AP32" t="s">
-        <v>172</v>
-      </c>
-      <c r="AQ32" t="s">
-        <v>174</v>
-      </c>
-      <c r="AR32" t="s">
-        <v>164</v>
-      </c>
-      <c r="AS32" t="s">
-        <v>164</v>
-      </c>
-      <c r="AT32" t="s">
-        <v>164</v>
-      </c>
-      <c r="AU32" t="s">
-        <v>164</v>
-      </c>
-      <c r="AV32" t="s">
-        <v>164</v>
-      </c>
-      <c r="AW32" t="s">
-        <v>164</v>
-      </c>
-      <c r="AX32" t="s">
-        <v>164</v>
-      </c>
-      <c r="AY32" t="s">
-        <v>164</v>
-      </c>
-      <c r="AZ32" t="s">
-        <v>164</v>
-      </c>
-      <c r="BA32" t="s">
-        <v>164</v>
-      </c>
-      <c r="BB32" t="s">
-        <v>164</v>
-      </c>
-      <c r="BC32" t="s">
-        <v>164</v>
-      </c>
-      <c r="BD32" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="33" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="34" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="35" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C35">
-        <v>15</v>
-      </c>
-      <c r="D35">
-        <v>15</v>
-      </c>
-      <c r="E35">
-        <v>15</v>
-      </c>
-      <c r="F35">
-        <v>15</v>
-      </c>
-      <c r="G35">
-        <v>15</v>
-      </c>
-      <c r="H35">
-        <v>15</v>
-      </c>
-      <c r="I35">
-        <v>15</v>
-      </c>
-      <c r="J35">
-        <v>15</v>
-      </c>
-      <c r="K35">
-        <v>15</v>
-      </c>
-      <c r="L35">
-        <v>15</v>
-      </c>
-      <c r="M35">
-        <v>15</v>
       </c>
       <c r="N35">
         <v>15</v>
@@ -15800,9 +16286,6 @@
       <c r="O35">
         <v>15</v>
       </c>
-      <c r="P35">
-        <v>15</v>
-      </c>
       <c r="Q35">
         <v>15</v>
       </c>
@@ -15815,6 +16298,33 @@
       <c r="T35">
         <v>15</v>
       </c>
+      <c r="U35">
+        <v>15</v>
+      </c>
+      <c r="V35">
+        <v>15</v>
+      </c>
+      <c r="X35">
+        <v>15</v>
+      </c>
+      <c r="Y35">
+        <v>15</v>
+      </c>
+      <c r="Z35">
+        <v>15</v>
+      </c>
+      <c r="AA35">
+        <v>15</v>
+      </c>
+      <c r="AB35">
+        <v>15</v>
+      </c>
+      <c r="AC35">
+        <v>15</v>
+      </c>
+      <c r="AE35">
+        <v>15</v>
+      </c>
       <c r="AF35">
         <v>15</v>
       </c>
@@ -15824,182 +16334,1176 @@
       <c r="AH35">
         <v>15</v>
       </c>
-      <c r="AI35">
+      <c r="BF35">
+        <v>15</v>
+      </c>
+      <c r="BG35">
+        <v>15</v>
+      </c>
+      <c r="BH35">
+        <v>15</v>
+      </c>
+      <c r="BI35">
         <v>14</v>
       </c>
-      <c r="AJ35">
+      <c r="BJ35">
         <v>14</v>
       </c>
-      <c r="AK35">
+      <c r="BL35">
         <v>15</v>
       </c>
-      <c r="AL35">
+      <c r="BM35">
         <v>15</v>
       </c>
-      <c r="AM35">
+      <c r="BN35">
         <v>15</v>
       </c>
-      <c r="AN35">
+      <c r="BO35">
         <v>15</v>
       </c>
-      <c r="AO35">
+      <c r="BP35">
         <v>15</v>
       </c>
-      <c r="AP35">
+      <c r="BQ35">
         <v>15</v>
       </c>
-      <c r="AQ35">
+      <c r="BS35">
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:89" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="AR36" t="s">
+        <v>169</v>
+      </c>
+      <c r="B36" t="s">
+        <v>220</v>
+      </c>
+      <c r="C36" t="s">
+        <v>228</v>
+      </c>
+      <c r="D36" t="s">
+        <v>228</v>
+      </c>
+      <c r="E36" t="s">
+        <v>228</v>
+      </c>
+      <c r="F36" t="s">
+        <v>220</v>
+      </c>
+      <c r="G36" t="s">
+        <v>220</v>
+      </c>
+      <c r="H36" t="s">
+        <v>220</v>
+      </c>
+      <c r="I36" t="s">
+        <v>228</v>
+      </c>
+      <c r="J36" t="s">
+        <v>220</v>
+      </c>
+      <c r="K36" t="s">
+        <v>220</v>
+      </c>
+      <c r="AM36" t="s">
+        <v>220</v>
+      </c>
+      <c r="AN36" t="s">
+        <v>220</v>
+      </c>
+      <c r="AO36" t="s">
+        <v>220</v>
+      </c>
+      <c r="BD36" t="s">
+        <v>220</v>
+      </c>
+      <c r="BE36" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="37" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J37" t="s">
+        <v>220</v>
+      </c>
+      <c r="K37" t="s">
+        <v>220</v>
+      </c>
+      <c r="L37" t="s">
+        <v>220</v>
+      </c>
+      <c r="M37" t="s">
+        <v>220</v>
+      </c>
+      <c r="W37" t="s">
+        <v>220</v>
+      </c>
+      <c r="AZ37" t="s">
+        <v>220</v>
+      </c>
+      <c r="BA37" t="s">
+        <v>220</v>
+      </c>
+      <c r="BB37" t="s">
+        <v>220</v>
+      </c>
+      <c r="BC37" t="s">
+        <v>220</v>
+      </c>
+      <c r="BD37" t="s">
+        <v>220</v>
+      </c>
+      <c r="BE37" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="38" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="BD38" t="s">
+        <v>274</v>
+      </c>
+      <c r="BE38" t="s">
+        <v>274</v>
+      </c>
+      <c r="BZ38" t="s">
+        <v>274</v>
+      </c>
+      <c r="CA38" t="s">
+        <v>274</v>
+      </c>
+      <c r="CB38" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="39" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="BD39" t="s">
+        <v>257</v>
+      </c>
+      <c r="BE39" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="40" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="P40" t="s">
+        <v>241</v>
+      </c>
+      <c r="BD40" t="s">
+        <v>241</v>
+      </c>
+      <c r="BE40" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="41" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="BD41" t="s">
+        <v>261</v>
+      </c>
+      <c r="BE41" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="42" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="BD42" t="s">
+        <v>275</v>
+      </c>
+      <c r="BE42" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="43" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B43" t="s">
+        <v>221</v>
+      </c>
+      <c r="C43" t="s">
+        <v>229</v>
+      </c>
+      <c r="D43" t="s">
+        <v>221</v>
+      </c>
+      <c r="E43" t="s">
+        <v>221</v>
+      </c>
+      <c r="F43" t="s">
+        <v>221</v>
+      </c>
+      <c r="G43" t="s">
+        <v>229</v>
+      </c>
+      <c r="H43" t="s">
+        <v>229</v>
+      </c>
+      <c r="I43" t="s">
+        <v>229</v>
+      </c>
+      <c r="AI43" t="s">
+        <v>229</v>
+      </c>
+      <c r="AJ43" t="s">
+        <v>255</v>
+      </c>
+      <c r="AM43" t="s">
+        <v>255</v>
+      </c>
+      <c r="AN43" t="s">
+        <v>263</v>
+      </c>
+      <c r="AO43" t="s">
+        <v>263</v>
+      </c>
+      <c r="AP43" t="s">
+        <v>221</v>
+      </c>
+      <c r="AQ43" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR43" t="s">
+        <v>255</v>
+      </c>
+      <c r="AS43" t="s">
+        <v>221</v>
+      </c>
+      <c r="AT43" t="s">
+        <v>229</v>
+      </c>
+      <c r="AU43" t="s">
+        <v>229</v>
+      </c>
+      <c r="AV43" t="s">
+        <v>255</v>
+      </c>
+      <c r="AW43" t="s">
+        <v>255</v>
+      </c>
+      <c r="AX43" t="s">
+        <v>229</v>
+      </c>
+      <c r="AY43" t="s">
+        <v>229</v>
+      </c>
+      <c r="BD43" t="s">
+        <v>263</v>
+      </c>
+      <c r="BE43" t="s">
+        <v>229</v>
+      </c>
+      <c r="BV43" t="s">
+        <v>282</v>
+      </c>
+      <c r="BW43" t="s">
+        <v>282</v>
+      </c>
+      <c r="BX43" t="s">
+        <v>283</v>
+      </c>
+      <c r="BY43" t="s">
+        <v>229</v>
+      </c>
+      <c r="BZ43" t="s">
+        <v>229</v>
+      </c>
+      <c r="CA43" t="s">
+        <v>283</v>
+      </c>
+      <c r="CB43" t="s">
+        <v>282</v>
+      </c>
+      <c r="CC43" t="s">
+        <v>229</v>
+      </c>
+      <c r="CD43" t="s">
+        <v>283</v>
+      </c>
+      <c r="CE43" t="s">
+        <v>229</v>
+      </c>
+      <c r="CF43" t="s">
+        <v>285</v>
+      </c>
+      <c r="CG43" t="s">
+        <v>229</v>
+      </c>
+      <c r="CH43" t="s">
+        <v>286</v>
+      </c>
+      <c r="CJ43" t="s">
+        <v>288</v>
+      </c>
+      <c r="CK43" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="44" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="BD44" t="s">
+        <v>276</v>
+      </c>
+      <c r="BE44" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="45" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="BK45" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="46" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="AZ46" t="s">
+        <v>269</v>
+      </c>
+      <c r="BA46" t="s">
+        <v>269</v>
+      </c>
+      <c r="BB46" t="s">
+        <v>269</v>
+      </c>
+      <c r="BC46" t="s">
+        <v>269</v>
+      </c>
+      <c r="BR46" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="47" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="AS36" t="s">
-        <v>180</v>
-      </c>
-      <c r="AT36" t="s">
+      <c r="B47" t="s">
+        <v>222</v>
+      </c>
+      <c r="C47" t="s">
+        <v>222</v>
+      </c>
+      <c r="D47" t="s">
+        <v>222</v>
+      </c>
+      <c r="E47" t="s">
+        <v>222</v>
+      </c>
+      <c r="F47" t="s">
+        <v>222</v>
+      </c>
+      <c r="G47" t="s">
+        <v>222</v>
+      </c>
+      <c r="H47" t="s">
+        <v>222</v>
+      </c>
+      <c r="I47" t="s">
+        <v>222</v>
+      </c>
+      <c r="L47" t="s">
+        <v>222</v>
+      </c>
+      <c r="M47" t="s">
+        <v>222</v>
+      </c>
+      <c r="AM47" t="s">
+        <v>222</v>
+      </c>
+      <c r="AN47" t="s">
+        <v>222</v>
+      </c>
+      <c r="AO47" t="s">
+        <v>222</v>
+      </c>
+      <c r="BR47" t="s">
+        <v>222</v>
+      </c>
+      <c r="BU47" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="48" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="AU36" t="s">
-        <v>180</v>
-      </c>
-      <c r="AV36" t="s">
-        <v>181</v>
-      </c>
-      <c r="AW36" t="s">
+      <c r="AM48" t="s">
+        <v>258</v>
+      </c>
+      <c r="AN48" t="s">
+        <v>258</v>
+      </c>
+      <c r="AO48" t="s">
+        <v>258</v>
+      </c>
+      <c r="BT48" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="49" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="AX36" t="s">
-        <v>182</v>
-      </c>
-      <c r="AY36" t="s">
-        <v>177</v>
-      </c>
-      <c r="AZ36" t="s">
-        <v>177</v>
-      </c>
-      <c r="BA36" t="s">
-        <v>181</v>
-      </c>
-      <c r="BB36" t="s">
-        <v>181</v>
-      </c>
-      <c r="BC36" t="s">
+      <c r="P49" t="s">
+        <v>242</v>
+      </c>
+      <c r="AI49" t="s">
+        <v>253</v>
+      </c>
+      <c r="AJ49" t="s">
+        <v>253</v>
+      </c>
+      <c r="AM49" t="s">
+        <v>257</v>
+      </c>
+      <c r="AN49" t="s">
+        <v>257</v>
+      </c>
+      <c r="AO49" t="s">
+        <v>257</v>
+      </c>
+      <c r="AP49" t="s">
+        <v>264</v>
+      </c>
+      <c r="AQ49" t="s">
+        <v>264</v>
+      </c>
+      <c r="AR49" t="s">
+        <v>264</v>
+      </c>
+      <c r="AS49" t="s">
+        <v>264</v>
+      </c>
+      <c r="AT49" t="s">
+        <v>264</v>
+      </c>
+      <c r="AU49" t="s">
+        <v>264</v>
+      </c>
+      <c r="AV49" t="s">
+        <v>264</v>
+      </c>
+      <c r="AW49" t="s">
+        <v>264</v>
+      </c>
+      <c r="AX49" t="s">
+        <v>264</v>
+      </c>
+      <c r="AY49" t="s">
+        <v>264</v>
+      </c>
+      <c r="BD49" t="s">
+        <v>257</v>
+      </c>
+      <c r="BE49" t="s">
+        <v>257</v>
+      </c>
+      <c r="BT49" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="50" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="BD36" t="s">
+      <c r="AL50" t="s">
+        <v>257</v>
+      </c>
+      <c r="BT50" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="51" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="37" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B37" t="s">
-        <v>165</v>
-      </c>
-      <c r="U37" t="s">
-        <v>176</v>
-      </c>
-      <c r="V37" t="s">
-        <v>176</v>
-      </c>
-      <c r="W37" t="s">
-        <v>178</v>
-      </c>
-      <c r="X37" t="s">
-        <v>178</v>
-      </c>
-      <c r="Y37" t="s">
-        <v>176</v>
-      </c>
-      <c r="Z37" t="s">
-        <v>165</v>
-      </c>
-      <c r="AA37" t="s">
-        <v>165</v>
-      </c>
-      <c r="AB37" t="s">
-        <v>176</v>
-      </c>
-      <c r="AC37" t="s">
-        <v>176</v>
-      </c>
-      <c r="AD37" t="s">
-        <v>176</v>
-      </c>
-      <c r="AE37" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="38" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="U38" t="s">
-        <v>177</v>
-      </c>
-      <c r="Y38" t="s">
-        <v>177</v>
-      </c>
-      <c r="Z38" t="s">
-        <v>177</v>
-      </c>
-      <c r="AA38" t="s">
-        <v>177</v>
-      </c>
-      <c r="AB38" t="s">
-        <v>177</v>
-      </c>
-      <c r="AC38" t="s">
-        <v>177</v>
-      </c>
-      <c r="AD38" t="s">
-        <v>177</v>
-      </c>
-      <c r="AE38" t="s">
-        <v>177</v>
-      </c>
-      <c r="AR38" t="s">
-        <v>177</v>
-      </c>
-      <c r="AS38" t="s">
-        <v>177</v>
-      </c>
-      <c r="AT38" t="s">
-        <v>177</v>
-      </c>
-      <c r="AU38" t="s">
-        <v>177</v>
-      </c>
-      <c r="AV38" t="s">
-        <v>177</v>
-      </c>
-      <c r="AW38" t="s">
-        <v>177</v>
-      </c>
-      <c r="AX38" t="s">
-        <v>177</v>
-      </c>
-      <c r="AY38" t="s">
-        <v>177</v>
-      </c>
-      <c r="AZ38" t="s">
-        <v>177</v>
-      </c>
-      <c r="BA38" t="s">
-        <v>177</v>
-      </c>
-      <c r="BB38" t="s">
-        <v>177</v>
-      </c>
-      <c r="BD38" t="s">
-        <v>177</v>
+      <c r="BU51" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="52" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="J52" t="s">
+        <v>230</v>
+      </c>
+      <c r="K52" t="s">
+        <v>230</v>
+      </c>
+      <c r="AP52" t="s">
+        <v>230</v>
+      </c>
+      <c r="AQ52" t="s">
+        <v>230</v>
+      </c>
+      <c r="AR52" t="s">
+        <v>230</v>
+      </c>
+      <c r="AS52" t="s">
+        <v>230</v>
+      </c>
+      <c r="AT52" t="s">
+        <v>230</v>
+      </c>
+      <c r="AU52" t="s">
+        <v>230</v>
+      </c>
+      <c r="AV52" t="s">
+        <v>230</v>
+      </c>
+      <c r="AW52" t="s">
+        <v>230</v>
+      </c>
+      <c r="AX52" t="s">
+        <v>230</v>
+      </c>
+      <c r="AY52" t="s">
+        <v>230</v>
+      </c>
+      <c r="BU52" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="53" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="J53" t="s">
+        <v>231</v>
+      </c>
+      <c r="K53" t="s">
+        <v>231</v>
+      </c>
+      <c r="BU53" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="54" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="BU54" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="55" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="BV55" t="s">
+        <v>231</v>
+      </c>
+      <c r="BW55" t="s">
+        <v>231</v>
+      </c>
+      <c r="BX55" t="s">
+        <v>231</v>
+      </c>
+      <c r="BY55" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="56" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="BZ56" t="s">
+        <v>275</v>
+      </c>
+      <c r="CA56" t="s">
+        <v>275</v>
+      </c>
+      <c r="CB56" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="57" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="BZ57" t="s">
+        <v>284</v>
+      </c>
+      <c r="CA57" t="s">
+        <v>284</v>
+      </c>
+      <c r="CB57" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="58" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B58" t="s">
+        <v>223</v>
+      </c>
+      <c r="C58" t="s">
+        <v>223</v>
+      </c>
+      <c r="D58" t="s">
+        <v>223</v>
+      </c>
+      <c r="E58" t="s">
+        <v>223</v>
+      </c>
+      <c r="F58" t="s">
+        <v>223</v>
+      </c>
+      <c r="G58" t="s">
+        <v>223</v>
+      </c>
+      <c r="H58" t="s">
+        <v>223</v>
+      </c>
+      <c r="I58" t="s">
+        <v>223</v>
+      </c>
+      <c r="CI58" t="s">
+        <v>287</v>
+      </c>
+      <c r="CL58" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="59" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="AI59" t="s">
+        <v>254</v>
+      </c>
+      <c r="AJ59" t="s">
+        <v>254</v>
+      </c>
+      <c r="CI59" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="60" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="AP60" t="s">
+        <v>265</v>
+      </c>
+      <c r="AQ60" t="s">
+        <v>265</v>
+      </c>
+      <c r="AR60" t="s">
+        <v>265</v>
+      </c>
+      <c r="AS60" t="s">
+        <v>265</v>
+      </c>
+      <c r="AT60" t="s">
+        <v>265</v>
+      </c>
+      <c r="AU60" t="s">
+        <v>265</v>
+      </c>
+      <c r="AV60" t="s">
+        <v>265</v>
+      </c>
+      <c r="AW60" t="s">
+        <v>265</v>
+      </c>
+      <c r="AX60" t="s">
+        <v>265</v>
+      </c>
+      <c r="AY60" t="s">
+        <v>265</v>
+      </c>
+      <c r="CL60" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="61" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="L61" t="s">
+        <v>235</v>
+      </c>
+      <c r="M61" t="s">
+        <v>235</v>
+      </c>
+      <c r="AI61" t="s">
+        <v>235</v>
+      </c>
+      <c r="AJ61" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="62" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="L62" t="s">
+        <v>236</v>
+      </c>
+      <c r="M62" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="63" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="L63" t="s">
+        <v>237</v>
+      </c>
+      <c r="M63" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD63" t="s">
+        <v>252</v>
+      </c>
+      <c r="AK63" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="64" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="L64" t="s">
+        <v>238</v>
+      </c>
+      <c r="M64" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="65" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P65" t="s">
+        <v>243</v>
+      </c>
+      <c r="AM65" t="s">
+        <v>259</v>
+      </c>
+      <c r="AN65" t="s">
+        <v>259</v>
+      </c>
+      <c r="AO65" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="66" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="W66" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="67" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AK67" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="68" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AM68" t="s">
+        <v>233</v>
+      </c>
+      <c r="AN68" t="s">
+        <v>233</v>
+      </c>
+      <c r="AO68" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="69" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="AM69" t="s">
+        <v>260</v>
+      </c>
+      <c r="AN69" t="s">
+        <v>260</v>
+      </c>
+      <c r="AO69" t="s">
+        <v>260</v>
+      </c>
+      <c r="AZ69" t="s">
+        <v>270</v>
+      </c>
+      <c r="BA69" t="s">
+        <v>270</v>
+      </c>
+      <c r="BB69" t="s">
+        <v>270</v>
+      </c>
+      <c r="BC69" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="70" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B70" t="s">
+        <v>224</v>
+      </c>
+      <c r="C70" t="s">
+        <v>224</v>
+      </c>
+      <c r="D70" t="s">
+        <v>224</v>
+      </c>
+      <c r="E70" t="s">
+        <v>224</v>
+      </c>
+      <c r="F70" t="s">
+        <v>224</v>
+      </c>
+      <c r="G70" t="s">
+        <v>224</v>
+      </c>
+      <c r="H70" t="s">
+        <v>224</v>
+      </c>
+      <c r="I70" t="s">
+        <v>224</v>
+      </c>
+      <c r="AM70" t="s">
+        <v>224</v>
+      </c>
+      <c r="AN70" t="s">
+        <v>224</v>
+      </c>
+      <c r="AO70" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="71" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="AM71" t="s">
+        <v>261</v>
+      </c>
+      <c r="AN71" t="s">
+        <v>261</v>
+      </c>
+      <c r="AO71" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="72" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="AM72" t="s">
+        <v>262</v>
+      </c>
+      <c r="AN72" t="s">
+        <v>262</v>
+      </c>
+      <c r="AO72" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="73" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AP73" t="s">
+        <v>266</v>
+      </c>
+      <c r="AQ73" t="s">
+        <v>266</v>
+      </c>
+      <c r="AR73" t="s">
+        <v>268</v>
+      </c>
+      <c r="AS73" t="s">
+        <v>268</v>
+      </c>
+      <c r="AT73" t="s">
+        <v>266</v>
+      </c>
+      <c r="AU73" t="s">
+        <v>268</v>
+      </c>
+      <c r="AV73" t="s">
+        <v>266</v>
+      </c>
+      <c r="AW73" t="s">
+        <v>268</v>
+      </c>
+      <c r="AX73" t="s">
+        <v>268</v>
+      </c>
+      <c r="AY73" t="s">
+        <v>266</v>
+      </c>
+      <c r="AZ73" t="s">
+        <v>271</v>
+      </c>
+      <c r="BA73" t="s">
+        <v>271</v>
+      </c>
+      <c r="BB73" t="s">
+        <v>271</v>
+      </c>
+      <c r="BC73" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="74" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="AP74" t="s">
+        <v>267</v>
+      </c>
+      <c r="AQ74" t="s">
+        <v>267</v>
+      </c>
+      <c r="AR74" t="s">
+        <v>267</v>
+      </c>
+      <c r="AS74" t="s">
+        <v>267</v>
+      </c>
+      <c r="AT74" t="s">
+        <v>267</v>
+      </c>
+      <c r="AU74" t="s">
+        <v>267</v>
+      </c>
+      <c r="AV74" t="s">
+        <v>267</v>
+      </c>
+      <c r="AW74" t="s">
+        <v>267</v>
+      </c>
+      <c r="AX74" t="s">
+        <v>267</v>
+      </c>
+      <c r="AY74" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="75" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="AZ75" t="s">
+        <v>272</v>
+      </c>
+      <c r="BA75" t="s">
+        <v>272</v>
+      </c>
+      <c r="BB75" t="s">
+        <v>272</v>
+      </c>
+      <c r="BC75" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="76" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="AZ76" t="s">
+        <v>269</v>
+      </c>
+      <c r="BA76" t="s">
+        <v>269</v>
+      </c>
+      <c r="BB76" t="s">
+        <v>269</v>
+      </c>
+      <c r="BC76" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="77" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="AZ77" t="s">
+        <v>273</v>
+      </c>
+      <c r="BA77" t="s">
+        <v>273</v>
+      </c>
+      <c r="BB77" t="s">
+        <v>273</v>
+      </c>
+      <c r="BC77" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="78" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="BD78" t="s">
+        <v>277</v>
+      </c>
+      <c r="BE78" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="79" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="BD79" t="s">
+        <v>231</v>
+      </c>
+      <c r="BE79" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="80" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B80" t="s">
+        <v>225</v>
+      </c>
+      <c r="C80" t="s">
+        <v>225</v>
+      </c>
+      <c r="D80" t="s">
+        <v>225</v>
+      </c>
+      <c r="E80" t="s">
+        <v>225</v>
+      </c>
+      <c r="F80" t="s">
+        <v>225</v>
+      </c>
+      <c r="G80" t="s">
+        <v>225</v>
+      </c>
+      <c r="H80" t="s">
+        <v>225</v>
+      </c>
+      <c r="I80" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B81" t="s">
+        <v>226</v>
+      </c>
+      <c r="C81" t="s">
+        <v>226</v>
+      </c>
+      <c r="D81" t="s">
+        <v>226</v>
+      </c>
+      <c r="E81" t="s">
+        <v>226</v>
+      </c>
+      <c r="F81" t="s">
+        <v>226</v>
+      </c>
+      <c r="G81" t="s">
+        <v>226</v>
+      </c>
+      <c r="H81" t="s">
+        <v>226</v>
+      </c>
+      <c r="I81" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B82" t="s">
+        <v>227</v>
+      </c>
+      <c r="C82" t="s">
+        <v>227</v>
+      </c>
+      <c r="D82" t="s">
+        <v>227</v>
+      </c>
+      <c r="E82" t="s">
+        <v>227</v>
+      </c>
+      <c r="F82" t="s">
+        <v>227</v>
+      </c>
+      <c r="G82" t="s">
+        <v>227</v>
+      </c>
+      <c r="H82" t="s">
+        <v>227</v>
+      </c>
+      <c r="I82" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="J83" t="s">
+        <v>232</v>
+      </c>
+      <c r="K83" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J84" t="s">
+        <v>233</v>
+      </c>
+      <c r="K84" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="J85" t="s">
+        <v>234</v>
+      </c>
+      <c r="K85" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>